<commit_message>
new results svm with BoW
</commit_message>
<xml_diff>
--- a/Grid search svm.xlsx
+++ b/Grid search svm.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Genevieve\Git\Analyse_dimage_avance_proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geneviève\Git\Analyse_dimage_avance_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Pixel" sheetId="1" r:id="rId1"/>
+    <sheet name="BoW" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>Hinge</t>
   </si>
@@ -98,21 +99,6 @@
     <t>Accuracy test 2</t>
   </si>
   <si>
-    <t>85.17</t>
-  </si>
-  <si>
-    <t>87.18</t>
-  </si>
-  <si>
-    <t>86.75</t>
-  </si>
-  <si>
-    <t>83.68</t>
-  </si>
-  <si>
-    <t>87.91</t>
-  </si>
-  <si>
     <t>{'loss': 'squared_hinge', 'C': 0.05, 'accuracy': 85.170000000000002, 'diff_accuracy': 1.1283333333333303}</t>
   </si>
   <si>
@@ -156,6 +142,21 @@
   </si>
   <si>
     <t>20-300</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result squared_hinge: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result hinge: </t>
   </si>
 </sst>
 </file>
@@ -205,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -268,11 +269,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
@@ -287,6 +325,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -296,8 +337,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3203,6 +3245,1176 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA"/>
+              <a:t>Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-CA" baseline="0"/>
+              <a:t> SVM</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Hinge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BoW!$A$22:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BoW!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>71.489999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83.894999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.456666666700002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84.921666666700006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.133333333300001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85.275000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85.428333333300003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85.518333333300006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.583333333300004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.613333333300005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85.616666666699999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>85.578333333299994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-9CC4-4C91-86C8-70C1A8EA0BD4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Squared Hinge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BoW!$A$22:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BoW!$B$22:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>79.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.108333333299996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85.323333333299999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85.473333333300005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85.488333333300005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85.493333333300001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85.496666666699994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.526666666699995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.553333333300003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85.431666666699996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>85.484999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-9CC4-4C91-86C8-70C1A8EA0BD4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="382008280"/>
+        <c:axId val="382008608"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="382008280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="382008608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="382008608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="86"/>
+          <c:min val="70"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="382008280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA"/>
+              <a:t>Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-CA" baseline="0"/>
+              <a:t> SVM</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Hinge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BoW!$I$2:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BoW!$J$2:$J$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>71.489999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.578333333299994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83.898333333300002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.458333333300004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84.918333333299998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.144999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85.28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85.348333333300005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85.421666666700006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85.525000000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.58</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.606666666699994</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85.625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>85.635000000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>85.601666666699998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85.583333333300004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85.575000000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85.586666666699998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-002C-4EB8-BF93-C3AC6E4DCABC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Squared Hinge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BoW!$I$2:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BoW!$J$22:$J$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>79.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.108333333299996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85.323333333299999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.438333333299994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85.473333333300005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85.488333333300005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85.495000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85.508333333300001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.515000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.52</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85.543333333299998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>85.5216666667</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>85.5366666667</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85.534999999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85.528333333299997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85.504999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-002C-4EB8-BF93-C3AC6E4DCABC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="382008280"/>
+        <c:axId val="382008608"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="382008280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="382008608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="382008608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="86"/>
+          <c:min val="70"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="382008280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3323,6 +4535,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4356,6 +5648,1038 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5056,6 +7380,73 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>190498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>596475</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>181498</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>710774</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5363,43 +7754,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="A48" sqref="A48:Q48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C2" s="9" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
       <c r="C3" s="2">
         <v>1</v>
@@ -5426,8 +7817,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -5458,8 +7849,8 @@
         <v>88.08</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="10"/>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -5488,36 +7879,36 @@
         <v>86.74</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C8" s="9" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
       <c r="C9" s="2">
         <v>1</v>
@@ -5544,8 +7935,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -5576,8 +7967,8 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="10"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
       <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
@@ -5606,7 +7997,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>6</v>
       </c>
@@ -5614,7 +8005,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>7</v>
       </c>
@@ -5622,7 +8013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>8</v>
       </c>
@@ -5630,7 +8021,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>9</v>
       </c>
@@ -5638,7 +8029,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>10</v>
       </c>
@@ -5646,7 +8037,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>11</v>
       </c>
@@ -5654,7 +8045,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>12</v>
       </c>
@@ -5662,7 +8053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>13</v>
       </c>
@@ -5670,7 +8061,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>14</v>
       </c>
@@ -5678,34 +8069,34 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="8" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C26" s="9" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
       <c r="C27" s="2">
         <v>0.5</v>
@@ -5726,8 +8117,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -5752,8 +8143,8 @@
         <v>84.04</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="10"/>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
       <c r="B29" s="4" t="s">
         <v>1</v>
       </c>
@@ -5776,34 +8167,34 @@
         <v>87.23</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C32" s="9" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
     </row>
-    <row r="33" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="3"/>
       <c r="C33" s="2">
         <v>0.5</v>
@@ -5824,8 +8215,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A34" s="10" t="s">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -5850,8 +8241,8 @@
         <v>0.61666666666699999</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A35" s="10"/>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
       <c r="B35" s="4" t="s">
         <v>1</v>
       </c>
@@ -5874,102 +8265,102 @@
         <v>0.87166666666699999</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="I41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="I42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+      <c r="I43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+      <c r="I44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>35</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
-        <v>36</v>
-      </c>
-      <c r="I41" t="s">
-        <v>30</v>
-      </c>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
-        <v>37</v>
-      </c>
-      <c r="I42" t="s">
-        <v>31</v>
-      </c>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C49" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
+      <c r="N49" s="12"/>
+      <c r="O49" s="12"/>
+      <c r="P49" s="12"/>
+      <c r="Q49" s="12"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
-        <v>38</v>
-      </c>
-      <c r="I43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
-        <v>39</v>
-      </c>
-      <c r="I44" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I45" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A48" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="C49" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
-      <c r="N49" s="9"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="9"/>
-      <c r="Q49" s="9"/>
-    </row>
-    <row r="50" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="3"/>
-      <c r="C50" s="11">
+      <c r="C50" s="8">
         <v>0.5</v>
       </c>
       <c r="D50" s="2">
@@ -6008,15 +8399,15 @@
       <c r="O50" s="2">
         <v>1000</v>
       </c>
-      <c r="P50" s="12">
+      <c r="P50" s="9">
         <v>2000</v>
       </c>
-      <c r="Q50" s="12">
+      <c r="Q50" s="9">
         <v>5000</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A51" s="10" t="s">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -6068,8 +8459,8 @@
         <v>86.56</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A52" s="10"/>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
       <c r="B52" s="4" t="s">
         <v>1</v>
       </c>
@@ -6119,52 +8510,52 @@
         <v>80.819999999999993</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A54" s="8" t="s">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="8"/>
-      <c r="N54" s="8"/>
-      <c r="O54" s="8"/>
-      <c r="P54" s="8"/>
-      <c r="Q54" s="8"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="11"/>
+      <c r="Q54" s="11"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="C55" s="9" t="s">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C55" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9"/>
-      <c r="L55" s="9"/>
-      <c r="M55" s="9"/>
-      <c r="N55" s="9"/>
-      <c r="O55" s="9"/>
-      <c r="P55" s="9"/>
-      <c r="Q55" s="9"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+      <c r="O55" s="12"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
     </row>
-    <row r="56" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="3"/>
-      <c r="C56" s="11">
+      <c r="C56" s="8">
         <v>0.5</v>
       </c>
       <c r="D56" s="2">
@@ -6203,15 +8594,15 @@
       <c r="O56" s="2">
         <v>1000</v>
       </c>
-      <c r="P56" s="12">
+      <c r="P56" s="9">
         <v>2000</v>
       </c>
-      <c r="Q56" s="12">
+      <c r="Q56" s="9">
         <v>5000</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="10" t="s">
+    <row r="57" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -6263,8 +8654,8 @@
         <v>1.25166666667</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A58" s="10"/>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
       <c r="B58" s="4" t="s">
         <v>1</v>
       </c>
@@ -6314,14 +8705,14 @@
         <v>1.57666666667</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K62" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -6445,4 +8836,1034 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="10"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1E-4</v>
+      </c>
+      <c r="B2" s="10">
+        <v>71.489999999999995</v>
+      </c>
+      <c r="C2" s="10">
+        <v>73.37</v>
+      </c>
+      <c r="D2" s="10">
+        <f>B2-C2</f>
+        <v>-1.8800000000000097</v>
+      </c>
+      <c r="I2">
+        <v>1E-4</v>
+      </c>
+      <c r="J2" s="10">
+        <v>71.489999999999995</v>
+      </c>
+      <c r="K2" s="10">
+        <v>73.38</v>
+      </c>
+      <c r="L2" s="10">
+        <f>J2-K2</f>
+        <v>-1.8900000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="B3" s="10">
+        <v>76.58</v>
+      </c>
+      <c r="C3" s="10">
+        <v>77.92</v>
+      </c>
+      <c r="D3" s="10">
+        <f t="shared" ref="D3:D15" si="0">B3-C3</f>
+        <v>-1.3400000000000034</v>
+      </c>
+      <c r="I3">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="J3" s="10">
+        <v>76.578333333299994</v>
+      </c>
+      <c r="K3" s="10">
+        <v>77.92</v>
+      </c>
+      <c r="L3" s="10">
+        <f t="shared" ref="L3:L19" si="1">J3-K3</f>
+        <v>-1.3416666667000072</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>83.894999999999996</v>
+      </c>
+      <c r="C4" s="10">
+        <v>83.92</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" si="0"/>
+        <v>-2.5000000000005684E-2</v>
+      </c>
+      <c r="I4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J4" s="10">
+        <v>83.898333333300002</v>
+      </c>
+      <c r="K4" s="10">
+        <v>83.92</v>
+      </c>
+      <c r="L4" s="10">
+        <f t="shared" si="1"/>
+        <v>-2.1666666699999837E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.01</v>
+      </c>
+      <c r="B5" s="10">
+        <v>84.456666666700002</v>
+      </c>
+      <c r="C5" s="10">
+        <v>84.45</v>
+      </c>
+      <c r="D5" s="10">
+        <f t="shared" si="0"/>
+        <v>6.6666666999992685E-3</v>
+      </c>
+      <c r="I5">
+        <v>0.01</v>
+      </c>
+      <c r="J5" s="10">
+        <v>84.458333333300004</v>
+      </c>
+      <c r="K5" s="10">
+        <v>84.45</v>
+      </c>
+      <c r="L5" s="10">
+        <f t="shared" si="1"/>
+        <v>8.3333333000012999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B6" s="10">
+        <v>84.921666666700006</v>
+      </c>
+      <c r="C6" s="10">
+        <v>84.89</v>
+      </c>
+      <c r="D6" s="10">
+        <f t="shared" si="0"/>
+        <v>3.1666666700004953E-2</v>
+      </c>
+      <c r="I6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J6" s="10">
+        <v>84.918333333299998</v>
+      </c>
+      <c r="K6" s="10">
+        <v>84.9</v>
+      </c>
+      <c r="L6" s="10">
+        <f t="shared" si="1"/>
+        <v>1.8333333299992205E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.05</v>
+      </c>
+      <c r="B7" s="10">
+        <v>85.133333333300001</v>
+      </c>
+      <c r="C7" s="10">
+        <v>85.13</v>
+      </c>
+      <c r="D7" s="10">
+        <f t="shared" si="0"/>
+        <v>3.3333333000058474E-3</v>
+      </c>
+      <c r="I7">
+        <v>0.05</v>
+      </c>
+      <c r="J7" s="10">
+        <v>85.144999999999996</v>
+      </c>
+      <c r="K7" s="10">
+        <v>85.1</v>
+      </c>
+      <c r="L7" s="10">
+        <f t="shared" si="1"/>
+        <v>4.5000000000001705E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B8" s="10">
+        <v>85.275000000000006</v>
+      </c>
+      <c r="C8" s="10">
+        <v>85.15</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="I8">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="J8" s="10">
+        <v>85.28</v>
+      </c>
+      <c r="K8" s="10">
+        <v>85.14</v>
+      </c>
+      <c r="L8" s="10">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000057</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.1</v>
+      </c>
+      <c r="B9" s="10">
+        <v>85.35</v>
+      </c>
+      <c r="C9" s="10">
+        <v>85.19</v>
+      </c>
+      <c r="D9" s="10">
+        <f t="shared" si="0"/>
+        <v>0.15999999999999659</v>
+      </c>
+      <c r="I9">
+        <v>0.1</v>
+      </c>
+      <c r="J9" s="10">
+        <v>85.348333333300005</v>
+      </c>
+      <c r="K9" s="10">
+        <v>85.17</v>
+      </c>
+      <c r="L9" s="10">
+        <f t="shared" si="1"/>
+        <v>0.17833333330000301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.2</v>
+      </c>
+      <c r="B10" s="10">
+        <v>85.428333333300003</v>
+      </c>
+      <c r="C10" s="10">
+        <v>85.23</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" si="0"/>
+        <v>0.19833333329999903</v>
+      </c>
+      <c r="I10">
+        <v>0.2</v>
+      </c>
+      <c r="J10" s="10">
+        <v>85.421666666700006</v>
+      </c>
+      <c r="K10" s="10">
+        <v>85.21</v>
+      </c>
+      <c r="L10" s="10">
+        <f t="shared" si="1"/>
+        <v>0.21166666670001177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.45</v>
+      </c>
+      <c r="B11" s="10">
+        <v>85.518333333300006</v>
+      </c>
+      <c r="C11" s="10">
+        <v>85.29</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="0"/>
+        <v>0.22833333330000016</v>
+      </c>
+      <c r="I11">
+        <v>0.45</v>
+      </c>
+      <c r="J11" s="10">
+        <v>85.525000000000006</v>
+      </c>
+      <c r="K11" s="10">
+        <v>85.33</v>
+      </c>
+      <c r="L11" s="10">
+        <f t="shared" si="1"/>
+        <v>0.19500000000000739</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.8</v>
+      </c>
+      <c r="B12" s="10">
+        <v>85.583333333300004</v>
+      </c>
+      <c r="C12" s="10">
+        <v>85.34</v>
+      </c>
+      <c r="D12" s="10">
+        <f t="shared" si="0"/>
+        <v>0.24333333330000073</v>
+      </c>
+      <c r="I12">
+        <v>0.8</v>
+      </c>
+      <c r="J12" s="10">
+        <v>85.58</v>
+      </c>
+      <c r="K12" s="10">
+        <v>85.34</v>
+      </c>
+      <c r="L12" s="10">
+        <f t="shared" si="1"/>
+        <v>0.23999999999999488</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="10">
+        <v>85.613333333300005</v>
+      </c>
+      <c r="C13" s="10">
+        <v>85.42</v>
+      </c>
+      <c r="D13" s="10">
+        <f t="shared" si="0"/>
+        <v>0.19333333330000357</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" s="10">
+        <v>85.606666666699994</v>
+      </c>
+      <c r="K13" s="10">
+        <v>85.36</v>
+      </c>
+      <c r="L13" s="10">
+        <f t="shared" si="1"/>
+        <v>0.24666666669999415</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1.5</v>
+      </c>
+      <c r="B14" s="10">
+        <v>85.616666666699999</v>
+      </c>
+      <c r="C14" s="10">
+        <v>85.35</v>
+      </c>
+      <c r="D14" s="10">
+        <f t="shared" si="0"/>
+        <v>0.26666666670000438</v>
+      </c>
+      <c r="I14">
+        <v>1.25</v>
+      </c>
+      <c r="J14" s="10">
+        <v>85.625</v>
+      </c>
+      <c r="K14" s="10">
+        <v>85.35</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" si="1"/>
+        <v>0.27500000000000568</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="10">
+        <v>85.578333333299994</v>
+      </c>
+      <c r="C15" s="10">
+        <v>85.32</v>
+      </c>
+      <c r="D15" s="10">
+        <f t="shared" si="0"/>
+        <v>0.2583333333000013</v>
+      </c>
+      <c r="I15" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="J15" s="15">
+        <v>85.635000000000005</v>
+      </c>
+      <c r="K15" s="15">
+        <v>85.36</v>
+      </c>
+      <c r="L15" s="16">
+        <f t="shared" si="1"/>
+        <v>0.27500000000000568</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>1.75</v>
+      </c>
+      <c r="J16" s="10">
+        <v>85.601666666699998</v>
+      </c>
+      <c r="K16" s="10">
+        <v>85.32</v>
+      </c>
+      <c r="L16" s="10">
+        <f t="shared" si="1"/>
+        <v>0.28166666670000495</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17" s="10">
+        <v>85.583333333300004</v>
+      </c>
+      <c r="K17" s="10">
+        <v>85.32</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="1"/>
+        <v>0.26333333330001096</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>2.5</v>
+      </c>
+      <c r="J18" s="10">
+        <v>85.575000000000003</v>
+      </c>
+      <c r="K18" s="10">
+        <v>85.27</v>
+      </c>
+      <c r="L18" s="10">
+        <f t="shared" si="1"/>
+        <v>0.30500000000000682</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19" s="10">
+        <v>85.586666666699998</v>
+      </c>
+      <c r="K19" s="10">
+        <v>85.28</v>
+      </c>
+      <c r="L19" s="10">
+        <f t="shared" si="1"/>
+        <v>0.30666666669999643</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1E-4</v>
+      </c>
+      <c r="B22" s="10">
+        <v>79.95</v>
+      </c>
+      <c r="C22" s="10">
+        <v>81.02</v>
+      </c>
+      <c r="D22" s="10">
+        <f>B22-C22</f>
+        <v>-1.0699999999999932</v>
+      </c>
+      <c r="I22">
+        <v>1E-4</v>
+      </c>
+      <c r="J22" s="10">
+        <v>79.95</v>
+      </c>
+      <c r="K22" s="10">
+        <v>81.02</v>
+      </c>
+      <c r="L22" s="10">
+        <f>J22-K22</f>
+        <v>-1.0699999999999932</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="B23" s="10">
+        <v>82.21</v>
+      </c>
+      <c r="C23" s="10">
+        <v>82.87</v>
+      </c>
+      <c r="D23" s="10">
+        <f t="shared" ref="D23:D34" si="2">B23-C23</f>
+        <v>-0.6600000000000108</v>
+      </c>
+      <c r="I23">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="J23" s="10">
+        <v>82.21</v>
+      </c>
+      <c r="K23" s="10">
+        <v>82.87</v>
+      </c>
+      <c r="L23" s="10">
+        <f t="shared" ref="L23:L39" si="3">J23-K23</f>
+        <v>-0.6600000000000108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B24" s="10">
+        <v>84.85</v>
+      </c>
+      <c r="C24" s="10">
+        <v>85.01</v>
+      </c>
+      <c r="D24" s="10">
+        <f t="shared" si="2"/>
+        <v>-0.1600000000000108</v>
+      </c>
+      <c r="I24">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J24" s="10">
+        <v>84.85</v>
+      </c>
+      <c r="K24" s="10">
+        <v>85.01</v>
+      </c>
+      <c r="L24" s="10">
+        <f t="shared" si="3"/>
+        <v>-0.1600000000000108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.01</v>
+      </c>
+      <c r="B25" s="10">
+        <v>85.108333333299996</v>
+      </c>
+      <c r="C25" s="10">
+        <v>85.35</v>
+      </c>
+      <c r="D25" s="10">
+        <f t="shared" si="2"/>
+        <v>-0.2416666666999987</v>
+      </c>
+      <c r="I25">
+        <v>0.01</v>
+      </c>
+      <c r="J25" s="10">
+        <v>85.108333333299996</v>
+      </c>
+      <c r="K25" s="10">
+        <v>85.35</v>
+      </c>
+      <c r="L25" s="10">
+        <f t="shared" si="3"/>
+        <v>-0.2416666666999987</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B26" s="10">
+        <v>85.323333333299999</v>
+      </c>
+      <c r="C26" s="10">
+        <v>85.33</v>
+      </c>
+      <c r="D26" s="10">
+        <f t="shared" si="2"/>
+        <v>-6.6666666999992685E-3</v>
+      </c>
+      <c r="I26">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J26" s="10">
+        <v>85.323333333299999</v>
+      </c>
+      <c r="K26" s="10">
+        <v>85.33</v>
+      </c>
+      <c r="L26" s="10">
+        <f t="shared" si="3"/>
+        <v>-6.6666666999992685E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.05</v>
+      </c>
+      <c r="B27" s="10">
+        <v>85.44</v>
+      </c>
+      <c r="C27" s="10">
+        <v>85.43</v>
+      </c>
+      <c r="D27" s="10">
+        <f t="shared" si="2"/>
+        <v>9.9999999999909051E-3</v>
+      </c>
+      <c r="I27">
+        <v>0.05</v>
+      </c>
+      <c r="J27" s="10">
+        <v>85.438333333299994</v>
+      </c>
+      <c r="K27" s="10">
+        <v>85.43</v>
+      </c>
+      <c r="L27" s="10">
+        <f t="shared" si="3"/>
+        <v>8.333333299987089E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B28" s="10">
+        <v>85.473333333300005</v>
+      </c>
+      <c r="C28" s="10">
+        <v>85.5</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" si="2"/>
+        <v>-2.6666666699995289E-2</v>
+      </c>
+      <c r="I28">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="J28" s="10">
+        <v>85.473333333300005</v>
+      </c>
+      <c r="K28" s="10">
+        <v>85.5</v>
+      </c>
+      <c r="L28" s="10">
+        <f t="shared" si="3"/>
+        <v>-2.6666666699995289E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.1</v>
+      </c>
+      <c r="B29" s="10">
+        <v>85.488333333300005</v>
+      </c>
+      <c r="C29" s="10">
+        <v>85.49</v>
+      </c>
+      <c r="D29" s="10">
+        <f t="shared" si="2"/>
+        <v>-1.6666666999896051E-3</v>
+      </c>
+      <c r="I29">
+        <v>0.1</v>
+      </c>
+      <c r="J29" s="10">
+        <v>85.488333333300005</v>
+      </c>
+      <c r="K29" s="10">
+        <v>85.49</v>
+      </c>
+      <c r="L29" s="10">
+        <f t="shared" si="3"/>
+        <v>-1.6666666999896051E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.2</v>
+      </c>
+      <c r="B30" s="10">
+        <v>85.493333333300001</v>
+      </c>
+      <c r="C30" s="10">
+        <v>85.51</v>
+      </c>
+      <c r="D30" s="10">
+        <f t="shared" si="2"/>
+        <v>-1.6666666700004384E-2</v>
+      </c>
+      <c r="I30">
+        <v>0.2</v>
+      </c>
+      <c r="J30" s="10">
+        <v>85.495000000000005</v>
+      </c>
+      <c r="K30" s="10">
+        <v>85.51</v>
+      </c>
+      <c r="L30" s="10">
+        <f t="shared" si="3"/>
+        <v>-1.5000000000000568E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.45</v>
+      </c>
+      <c r="B31" s="10">
+        <v>85.496666666699994</v>
+      </c>
+      <c r="C31" s="10">
+        <v>85.46</v>
+      </c>
+      <c r="D31" s="10">
+        <f t="shared" si="2"/>
+        <v>3.6666666700000405E-2</v>
+      </c>
+      <c r="I31">
+        <v>0.45</v>
+      </c>
+      <c r="J31" s="10">
+        <v>85.508333333300001</v>
+      </c>
+      <c r="K31" s="10">
+        <v>85.5</v>
+      </c>
+      <c r="L31" s="10">
+        <f t="shared" si="3"/>
+        <v>8.3333333000012999E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.8</v>
+      </c>
+      <c r="B32" s="10">
+        <v>85.526666666699995</v>
+      </c>
+      <c r="C32" s="10">
+        <v>85.5</v>
+      </c>
+      <c r="D32" s="10">
+        <f t="shared" si="2"/>
+        <v>2.6666666699995289E-2</v>
+      </c>
+      <c r="I32">
+        <v>0.8</v>
+      </c>
+      <c r="J32" s="10">
+        <v>85.515000000000001</v>
+      </c>
+      <c r="K32" s="10">
+        <v>85.52</v>
+      </c>
+      <c r="L32" s="10">
+        <f t="shared" si="3"/>
+        <v>-4.9999999999954525E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" s="10">
+        <v>85.553333333300003</v>
+      </c>
+      <c r="C33" s="10">
+        <v>85.52</v>
+      </c>
+      <c r="D33" s="10">
+        <f t="shared" si="2"/>
+        <v>3.3333333300006984E-2</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" s="10">
+        <v>85.52</v>
+      </c>
+      <c r="K33" s="10">
+        <v>85.51</v>
+      </c>
+      <c r="L33" s="10">
+        <f t="shared" si="3"/>
+        <v>9.9999999999909051E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1.5</v>
+      </c>
+      <c r="B34" s="10">
+        <v>85.431666666699996</v>
+      </c>
+      <c r="C34" s="10">
+        <v>85.43</v>
+      </c>
+      <c r="D34" s="10">
+        <f t="shared" si="2"/>
+        <v>1.6666666999896051E-3</v>
+      </c>
+      <c r="I34">
+        <v>1.25</v>
+      </c>
+      <c r="J34" s="10">
+        <v>85.543333333299998</v>
+      </c>
+      <c r="K34" s="10">
+        <v>85.51</v>
+      </c>
+      <c r="L34" s="10">
+        <f t="shared" si="3"/>
+        <v>3.3333333299992773E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" s="10">
+        <v>85.484999999999999</v>
+      </c>
+      <c r="C35" s="10">
+        <v>85.3</v>
+      </c>
+      <c r="D35" s="10">
+        <f>B35-C35</f>
+        <v>0.18500000000000227</v>
+      </c>
+      <c r="I35">
+        <v>1.5</v>
+      </c>
+      <c r="J35" s="10">
+        <v>85.5216666667</v>
+      </c>
+      <c r="K35" s="10">
+        <v>85.51</v>
+      </c>
+      <c r="L35" s="10">
+        <f t="shared" si="3"/>
+        <v>1.1666666699994721E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>1.75</v>
+      </c>
+      <c r="J36" s="10">
+        <v>85.5366666667</v>
+      </c>
+      <c r="K36" s="10">
+        <v>85.5</v>
+      </c>
+      <c r="L36" s="10">
+        <f t="shared" si="3"/>
+        <v>3.6666666700000405E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37" s="10">
+        <v>85.534999999999997</v>
+      </c>
+      <c r="K37" s="10">
+        <v>85.56</v>
+      </c>
+      <c r="L37" s="10">
+        <f t="shared" si="3"/>
+        <v>-2.5000000000005684E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>2.5</v>
+      </c>
+      <c r="J38" s="10">
+        <v>85.528333333299997</v>
+      </c>
+      <c r="K38" s="10">
+        <v>85.55</v>
+      </c>
+      <c r="L38" s="10">
+        <f t="shared" si="3"/>
+        <v>-2.1666666699999837E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="J39" s="10">
+        <v>85.504999999999995</v>
+      </c>
+      <c r="K39" s="10">
+        <v>85.49</v>
+      </c>
+      <c r="L39" s="10">
+        <f t="shared" si="3"/>
+        <v>1.5000000000000568E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B22:B35 B2:B15">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C35 C2:C15">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J19 J22:J39">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22:K39 K2:K19">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
-new result with hog -change code for make cross-validation and confusion matrix
</commit_message>
<xml_diff>
--- a/Grid search svm.xlsx
+++ b/Grid search svm.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Pixel" sheetId="3" r:id="rId1"/>
     <sheet name="BoW" sheetId="2" r:id="rId2"/>
     <sheet name="HoG" sheetId="4" r:id="rId3"/>
+    <sheet name="HoG2" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="5">
   <si>
     <t>Test</t>
   </si>
@@ -3612,6 +3613,626 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="70"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="382008280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA"/>
+              <a:t>Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-CA" baseline="0"/>
+              <a:t> SVM</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Hinge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'HoG2'!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>9.9999999999999995E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HoG2'!$B$2:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>90.851666666699998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.993333333300001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.506666666699999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92.751666666700004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.883333333300001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88.901666666699995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.878333333300006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.073333333299999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>86.591666666699993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85.803333333300003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>88.5216666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>87.363333333300005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85.655000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>83.986666666700003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>88.108333333299996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>84.811666666700006</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>89.186666666700006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>89.541666666699996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89.336666666699998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A71-4671-BF3C-0F9FC6131AE6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Squared Hinge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'HoG2'!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>9.9999999999999995E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HoG2'!$B$23:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>91.421666666700006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>92.008333333300001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91.17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.493333333300001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87.601666666699998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>86.454999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.325000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88.031666666700005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>87.763333333299997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>87.8533333333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>88.438333333299994</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>87.456666666700002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>84.5366666667</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87.616666666699999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87.281666666700005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>87.336666666699998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88.083333333300004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>85.921666666700006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7A71-4671-BF3C-0F9FC6131AE6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="382008280"/>
+        <c:axId val="382008608"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="382008280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="382008608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="382008608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="82"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4010,6 +4631,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -6591,6 +7252,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7303,6 +8480,43 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>748875</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>10050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7610,7 +8824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9772,7 +10986,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:T41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10894,4 +12110,650 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>90.851666666699998</v>
+      </c>
+      <c r="C2" s="1">
+        <v>91.41</v>
+      </c>
+      <c r="D2" s="1">
+        <f>B2-C2</f>
+        <v>-0.55833333329999846</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>91.993333333300001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>91.95</v>
+      </c>
+      <c r="D3" s="1">
+        <f>B3-C3</f>
+        <v>4.3333333299997889E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>92.506666666699999</v>
+      </c>
+      <c r="C4" s="1">
+        <v>92.03</v>
+      </c>
+      <c r="D4" s="1">
+        <f>B4-C4</f>
+        <v>0.47666666669999813</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>1E-4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>92.751666666700004</v>
+      </c>
+      <c r="C5" s="1">
+        <v>92.01</v>
+      </c>
+      <c r="D5" s="1">
+        <f>B5-C5</f>
+        <v>0.7416666666999987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>91.883333333300001</v>
+      </c>
+      <c r="C6" s="1">
+        <v>90.69</v>
+      </c>
+      <c r="D6" s="1">
+        <f>B6-C6</f>
+        <v>1.1933333333000036</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>88.901666666699995</v>
+      </c>
+      <c r="C7" s="1">
+        <v>87.99</v>
+      </c>
+      <c r="D7" s="1">
+        <f>B7-C7</f>
+        <v>0.91166666670000041</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="B8" s="1">
+        <v>88.878333333300006</v>
+      </c>
+      <c r="C8" s="1">
+        <v>88.3</v>
+      </c>
+      <c r="D8" s="1">
+        <f>B8-C8</f>
+        <v>0.57833333330000869</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>88.073333333299999</v>
+      </c>
+      <c r="C9" s="1">
+        <v>87.36</v>
+      </c>
+      <c r="D9" s="1">
+        <f>B9-C9</f>
+        <v>0.71333333329999959</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="B10" s="1">
+        <v>86.591666666699993</v>
+      </c>
+      <c r="C10" s="1">
+        <v>85.76</v>
+      </c>
+      <c r="D10" s="1">
+        <f>B10-C10</f>
+        <v>0.8316666666999879</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>85.803333333300003</v>
+      </c>
+      <c r="C11" s="1">
+        <v>84.19</v>
+      </c>
+      <c r="D11" s="1">
+        <f>B11-C11</f>
+        <v>1.6133333333000053</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>88.5216666667</v>
+      </c>
+      <c r="C12" s="1">
+        <v>87.71</v>
+      </c>
+      <c r="D12" s="1">
+        <f>B12-C12</f>
+        <v>0.81166666670000609</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>87.363333333300005</v>
+      </c>
+      <c r="C13" s="1">
+        <v>86.36</v>
+      </c>
+      <c r="D13" s="1">
+        <f>B13-C13</f>
+        <v>1.0033333333000058</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="B14" s="1">
+        <v>85.655000000000001</v>
+      </c>
+      <c r="C14" s="1">
+        <v>84.88</v>
+      </c>
+      <c r="D14" s="1">
+        <f>B14-C14</f>
+        <v>0.77500000000000568</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="B15" s="1">
+        <v>83.986666666700003</v>
+      </c>
+      <c r="C15" s="1">
+        <v>83.51</v>
+      </c>
+      <c r="D15" s="1">
+        <f>B15-C15</f>
+        <v>0.47666666669999813</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>88.108333333299996</v>
+      </c>
+      <c r="C16" s="1">
+        <v>87.11</v>
+      </c>
+      <c r="D16" s="1">
+        <f>B16-C16</f>
+        <v>0.99833333329999618</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="B17" s="1">
+        <v>84.811666666700006</v>
+      </c>
+      <c r="C17" s="1">
+        <v>83.24</v>
+      </c>
+      <c r="D17" s="1">
+        <f>B17-C17</f>
+        <v>1.5716666667000112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="B18" s="1">
+        <v>89.186666666700006</v>
+      </c>
+      <c r="C18" s="1">
+        <v>88.43</v>
+      </c>
+      <c r="D18" s="1">
+        <f>B18-C18</f>
+        <v>0.75666666669999927</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="B19" s="1">
+        <v>89.541666666699996</v>
+      </c>
+      <c r="C19" s="1">
+        <v>88.62</v>
+      </c>
+      <c r="D19" s="1">
+        <f>B19-C19</f>
+        <v>0.92166666669999131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1">
+        <v>89.336666666699998</v>
+      </c>
+      <c r="C20" s="1">
+        <v>88.68</v>
+      </c>
+      <c r="D20" s="1">
+        <f>B20-C20</f>
+        <v>0.65666666669999074</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="B23" s="1">
+        <v>91.421666666700006</v>
+      </c>
+      <c r="C23" s="1">
+        <v>91.38</v>
+      </c>
+      <c r="D23" s="1">
+        <f>B23-C23</f>
+        <v>4.1666666700010069E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="B24" s="1">
+        <v>92.008333333300001</v>
+      </c>
+      <c r="C24" s="1">
+        <v>91.67</v>
+      </c>
+      <c r="D24" s="1">
+        <f>B24-C24</f>
+        <v>0.33833333329999959</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="B25" s="1">
+        <v>92.26</v>
+      </c>
+      <c r="C25" s="1">
+        <v>91.75</v>
+      </c>
+      <c r="D25" s="1">
+        <f>B25-C25</f>
+        <v>0.51000000000000512</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>1E-4</v>
+      </c>
+      <c r="B26" s="1">
+        <v>91.17</v>
+      </c>
+      <c r="C26" s="1">
+        <v>90.55</v>
+      </c>
+      <c r="D26" s="1">
+        <f>B26-C26</f>
+        <v>0.62000000000000455</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="B27" s="1">
+        <v>90.493333333300001</v>
+      </c>
+      <c r="C27" s="1">
+        <v>90.02</v>
+      </c>
+      <c r="D27" s="1">
+        <f>B27-C27</f>
+        <v>0.47333333330000471</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B28" s="1">
+        <v>87.601666666699998</v>
+      </c>
+      <c r="C28" s="1">
+        <v>86.69</v>
+      </c>
+      <c r="D28" s="1">
+        <f>B28-C28</f>
+        <v>0.91166666670000041</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="B29" s="1">
+        <v>86.454999999999998</v>
+      </c>
+      <c r="C29" s="1">
+        <v>86.1</v>
+      </c>
+      <c r="D29" s="1">
+        <f>B29-C29</f>
+        <v>0.35500000000000398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B30" s="1">
+        <v>88.325000000000003</v>
+      </c>
+      <c r="C30" s="1">
+        <v>87.59</v>
+      </c>
+      <c r="D30" s="1">
+        <f>B30-C30</f>
+        <v>0.73499999999999943</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="B31" s="1">
+        <v>88.031666666700005</v>
+      </c>
+      <c r="C31" s="1">
+        <v>86.88</v>
+      </c>
+      <c r="D31" s="1">
+        <f>B31-C31</f>
+        <v>1.1516666667000095</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B32" s="1">
+        <v>87.763333333299997</v>
+      </c>
+      <c r="C32" s="1">
+        <v>87.18</v>
+      </c>
+      <c r="D32" s="1">
+        <f>B32-C32</f>
+        <v>0.58333333329998993</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="B33" s="1">
+        <v>87.8533333333</v>
+      </c>
+      <c r="C33" s="1">
+        <v>87.07</v>
+      </c>
+      <c r="D33" s="1">
+        <f>B33-C33</f>
+        <v>0.78333333330000698</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="B34" s="1">
+        <v>88.438333333299994</v>
+      </c>
+      <c r="C34" s="1">
+        <v>88.05</v>
+      </c>
+      <c r="D34" s="1">
+        <f>B34-C34</f>
+        <v>0.38833333329999675</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="B35" s="1">
+        <v>87.456666666700002</v>
+      </c>
+      <c r="C35" s="1">
+        <v>86.81</v>
+      </c>
+      <c r="D35" s="1">
+        <f>B35-C35</f>
+        <v>0.64666666669999984</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="B36" s="1">
+        <v>84.5366666667</v>
+      </c>
+      <c r="C36" s="1">
+        <v>84.23</v>
+      </c>
+      <c r="D36" s="1">
+        <f>B36-C36</f>
+        <v>0.30666666669999643</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1">
+        <v>87.616666666699999</v>
+      </c>
+      <c r="C37" s="1">
+        <v>86.7</v>
+      </c>
+      <c r="D37" s="1">
+        <f>B37-C37</f>
+        <v>0.91666666669999586</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="B38" s="1">
+        <v>87.281666666700005</v>
+      </c>
+      <c r="C38" s="1">
+        <v>86.4</v>
+      </c>
+      <c r="D38" s="1">
+        <f>B38-C38</f>
+        <v>0.88166666669999927</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="B39" s="1">
+        <v>87.336666666699998</v>
+      </c>
+      <c r="C39" s="1">
+        <v>86.48</v>
+      </c>
+      <c r="D39" s="1">
+        <f>B39-C39</f>
+        <v>0.85666666669999358</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="B40" s="1">
+        <v>88.083333333300004</v>
+      </c>
+      <c r="C40" s="1">
+        <v>87.51</v>
+      </c>
+      <c r="D40" s="1">
+        <f>B40-C40</f>
+        <v>0.57333333329999903</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1">
+        <v>85.921666666700006</v>
+      </c>
+      <c r="C41" s="1">
+        <v>86.24</v>
+      </c>
+      <c r="D41" s="1">
+        <f>B41-C41</f>
+        <v>-0.31833333329998936</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B23:B41 B2:B20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23:C41 C2:C20">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
-correct svm to compute cross-validation and get best result of feature for real test with good C and loss -correct svm to create matrix confusion
</commit_message>
<xml_diff>
--- a/Grid search svm.xlsx
+++ b/Grid search svm.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="7">
   <si>
     <t>Test</t>
   </si>
@@ -20620,9 +20620,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ51"/>
+  <dimension ref="A1:AR51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AE31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AQ20" sqref="AQ20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20638,9 +20640,11 @@
     <col min="26" max="28" width="11.42578125" style="1"/>
     <col min="33" max="33" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="34" max="36" width="11.42578125" style="1"/>
+    <col min="41" max="41" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="44" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -20704,8 +20708,20 @@
       <c r="AJ1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="AO1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -20767,8 +20783,20 @@
       <c r="AJ2" s="1">
         <v>-1.89</v>
       </c>
+      <c r="AO2">
+        <v>1E-4</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>73.033333333300007</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>73.722222222200003</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>-0.68888888888900002</v>
+      </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -20829,8 +20857,20 @@
       <c r="AJ3" s="1">
         <v>-0.54500000000000004</v>
       </c>
+      <c r="AO3">
+        <v>1E-3</v>
+      </c>
+      <c r="AP3" s="1">
+        <v>72.716666666699993</v>
+      </c>
+      <c r="AQ3" s="1">
+        <v>73.327777777799994</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>-0.61111111111100003</v>
+      </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -20891,8 +20931,20 @@
       <c r="AJ4" s="1">
         <v>6.6666666666599997E-3</v>
       </c>
+      <c r="AO4">
+        <v>0.01</v>
+      </c>
+      <c r="AP4" s="1">
+        <v>79.940476190499993</v>
+      </c>
+      <c r="AQ4" s="1">
+        <v>80.366666666699999</v>
+      </c>
+      <c r="AR4" s="1">
+        <v>-0.42619047619</v>
+      </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -20953,8 +21005,20 @@
       <c r="AJ5" s="1">
         <v>0.148333333333</v>
       </c>
+      <c r="AO5">
+        <v>0.1</v>
+      </c>
+      <c r="AP5" s="1">
+        <v>86.135714285700004</v>
+      </c>
+      <c r="AQ5" s="1">
+        <v>86.144444444399994</v>
+      </c>
+      <c r="AR5" s="1">
+        <v>-8.7301587301600002E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -21015,8 +21079,20 @@
       <c r="AJ6" s="1">
         <v>0.226666666667</v>
       </c>
+      <c r="AO6">
+        <v>0.5</v>
+      </c>
+      <c r="AP6" s="1">
+        <v>86.919047618999997</v>
+      </c>
+      <c r="AQ6" s="1">
+        <v>87</v>
+      </c>
+      <c r="AR6" s="1">
+        <v>-8.0952380952399997E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
@@ -21077,8 +21153,20 @@
       <c r="AJ7" s="1">
         <v>0.28166666666700002</v>
       </c>
+      <c r="AO7">
+        <v>1</v>
+      </c>
+      <c r="AP7" s="1">
+        <v>87.05</v>
+      </c>
+      <c r="AQ7" s="1">
+        <v>87.155555555600003</v>
+      </c>
+      <c r="AR7" s="1">
+        <v>-0.10555555555600001</v>
+      </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>25</v>
       </c>
@@ -21139,8 +21227,20 @@
       <c r="AJ8" s="1">
         <v>0.34333333333299998</v>
       </c>
+      <c r="AO8">
+        <v>1.5</v>
+      </c>
+      <c r="AP8" s="1">
+        <v>87.088095238099996</v>
+      </c>
+      <c r="AQ8" s="1">
+        <v>87.177777777800003</v>
+      </c>
+      <c r="AR8" s="1">
+        <v>-8.9682539682500007E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>30</v>
       </c>
@@ -21201,8 +21301,20 @@
       <c r="AJ9" s="1">
         <v>0.25166666666699999</v>
       </c>
+      <c r="AO9">
+        <v>2</v>
+      </c>
+      <c r="AP9" s="1">
+        <v>87.135714285700004</v>
+      </c>
+      <c r="AQ9" s="1">
+        <v>87.255555555599997</v>
+      </c>
+      <c r="AR9" s="1">
+        <v>-0.11984126984100001</v>
+      </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -21263,8 +21375,20 @@
       <c r="AJ10" s="1">
         <v>0.29333333333299999</v>
       </c>
+      <c r="AO10">
+        <v>2.5</v>
+      </c>
+      <c r="AP10" s="1">
+        <v>87.169047618999997</v>
+      </c>
+      <c r="AQ10" s="1">
+        <v>87.244444444400003</v>
+      </c>
+      <c r="AR10" s="1">
+        <v>-7.5396825396799996E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>50</v>
       </c>
@@ -21325,8 +21449,20 @@
       <c r="AJ11" s="1">
         <v>0.256666666667</v>
       </c>
+      <c r="AO11">
+        <v>3</v>
+      </c>
+      <c r="AP11" s="1">
+        <v>87.202380952400006</v>
+      </c>
+      <c r="AQ11" s="1">
+        <v>87.244444444400003</v>
+      </c>
+      <c r="AR11" s="1">
+        <v>-4.2063492063499998E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>60</v>
       </c>
@@ -21387,8 +21523,20 @@
       <c r="AJ12" s="1">
         <v>0.28166666666700002</v>
       </c>
+      <c r="AO12">
+        <v>3.5</v>
+      </c>
+      <c r="AP12" s="1">
+        <v>87.207142857099996</v>
+      </c>
+      <c r="AQ12" s="1">
+        <v>87.25</v>
+      </c>
+      <c r="AR12" s="1">
+        <v>-4.2857142857100003E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>70</v>
       </c>
@@ -21449,8 +21597,20 @@
       <c r="AJ13" s="1">
         <v>0.238333333333</v>
       </c>
+      <c r="AO13">
+        <v>4</v>
+      </c>
+      <c r="AP13" s="1">
+        <v>87.228571428600006</v>
+      </c>
+      <c r="AQ13" s="1">
+        <v>87.288888888900004</v>
+      </c>
+      <c r="AR13" s="1">
+        <v>-6.0317460317500002E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>80</v>
       </c>
@@ -21511,8 +21671,20 @@
       <c r="AJ14" s="1">
         <v>0.45333333333300002</v>
       </c>
+      <c r="AO14">
+        <v>4.5</v>
+      </c>
+      <c r="AP14" s="1">
+        <v>87.238095238100001</v>
+      </c>
+      <c r="AQ14" s="1">
+        <v>87.316666666700002</v>
+      </c>
+      <c r="AR14" s="1">
+        <v>-7.8571428571399995E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>90</v>
       </c>
@@ -21573,8 +21745,20 @@
       <c r="AJ15" s="1">
         <v>0.36666666666699999</v>
       </c>
+      <c r="AO15">
+        <v>5</v>
+      </c>
+      <c r="AP15" s="1">
+        <v>87.240476190500004</v>
+      </c>
+      <c r="AQ15" s="1">
+        <v>87.305555555599994</v>
+      </c>
+      <c r="AR15" s="1">
+        <v>-6.5079365079400001E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>100</v>
       </c>
@@ -21635,8 +21819,20 @@
       <c r="AJ16" s="1">
         <v>0.28333333333299998</v>
       </c>
+      <c r="AO16">
+        <v>6</v>
+      </c>
+      <c r="AP16" s="1">
+        <v>87.240476190500004</v>
+      </c>
+      <c r="AQ16" s="1">
+        <v>87.2944444444</v>
+      </c>
+      <c r="AR16" s="1">
+        <v>-5.3968253968300003E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>150</v>
       </c>
@@ -21697,8 +21893,20 @@
       <c r="AJ17" s="1">
         <v>0.54333333333300005</v>
       </c>
+      <c r="AO17">
+        <v>7</v>
+      </c>
+      <c r="AP17" s="1">
+        <v>87.245238095199994</v>
+      </c>
+      <c r="AQ17" s="1">
+        <v>87.333333333300004</v>
+      </c>
+      <c r="AR17" s="1">
+        <v>-8.8095238095200007E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>200</v>
       </c>
@@ -21759,8 +21967,20 @@
       <c r="AJ18" s="1">
         <v>0.488333333333</v>
       </c>
+      <c r="AO18">
+        <v>8</v>
+      </c>
+      <c r="AP18" s="1">
+        <v>87.240476190500004</v>
+      </c>
+      <c r="AQ18" s="1">
+        <v>87.333333333300004</v>
+      </c>
+      <c r="AR18" s="1">
+        <v>-9.2857142857100006E-2</v>
+      </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>250</v>
       </c>
@@ -21809,8 +22029,20 @@
       <c r="AJ19" s="1">
         <v>0.28833333333299999</v>
       </c>
+      <c r="AO19">
+        <v>9</v>
+      </c>
+      <c r="AP19" s="1">
+        <v>87.245238095199994</v>
+      </c>
+      <c r="AQ19" s="1">
+        <v>87.383333333300001</v>
+      </c>
+      <c r="AR19" s="1">
+        <v>-0.13809523809499999</v>
+      </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>300</v>
       </c>
@@ -21859,8 +22091,20 @@
       <c r="AJ20" s="1">
         <v>0.36</v>
       </c>
+      <c r="AO20">
+        <v>10</v>
+      </c>
+      <c r="AP20" s="1">
+        <v>87.261904761899999</v>
+      </c>
+      <c r="AQ20" s="1">
+        <v>87.405555555600003</v>
+      </c>
+      <c r="AR20" s="1">
+        <v>-0.143650793651</v>
+      </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>350</v>
       </c>
@@ -21909,8 +22153,20 @@
       <c r="AJ21" s="1">
         <v>0.45166666666700001</v>
       </c>
+      <c r="AO21">
+        <v>15</v>
+      </c>
+      <c r="AP21" s="1">
+        <v>87.307142857100004</v>
+      </c>
+      <c r="AQ21" s="1">
+        <v>87.383333333300001</v>
+      </c>
+      <c r="AR21" s="1">
+        <v>-7.6190476190499998E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>400</v>
       </c>
@@ -21924,7 +22180,7 @@
         <v>-0.386666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>450</v>
       </c>
@@ -21938,7 +22194,7 @@
         <v>-0.96666666666699996</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>500</v>
       </c>
@@ -21952,7 +22208,7 @@
         <v>-0.13333333333299999</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1000</v>
       </c>
@@ -21966,7 +22222,7 @@
         <v>-0.103333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -22027,8 +22283,20 @@
       <c r="AJ27" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="AO27" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR27" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="28" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -22089,8 +22357,20 @@
       <c r="AJ28" s="1">
         <v>-1.07</v>
       </c>
+      <c r="AO28">
+        <v>1E-4</v>
+      </c>
+      <c r="AP28" s="1">
+        <v>67.140476190499996</v>
+      </c>
+      <c r="AQ28" s="1">
+        <v>67.55</v>
+      </c>
+      <c r="AR28" s="1">
+        <v>-0.40952380952400003</v>
+      </c>
     </row>
-    <row r="29" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>3</v>
       </c>
@@ -22151,8 +22431,20 @@
       <c r="AJ29" s="1">
         <v>-0.34499999999999997</v>
       </c>
+      <c r="AO29">
+        <v>1E-3</v>
+      </c>
+      <c r="AP29" s="1">
+        <v>80.566666666700002</v>
+      </c>
+      <c r="AQ29" s="1">
+        <v>81</v>
+      </c>
+      <c r="AR29" s="1">
+        <v>-0.433333333333</v>
+      </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -22213,8 +22505,20 @@
       <c r="AJ30" s="1">
         <v>-0.24166666666700001</v>
       </c>
+      <c r="AO30">
+        <v>0.01</v>
+      </c>
+      <c r="AP30" s="1">
+        <v>85.461904761900001</v>
+      </c>
+      <c r="AQ30" s="1">
+        <v>85.538888888900004</v>
+      </c>
+      <c r="AR30" s="1">
+        <v>-7.6984126984099996E-2</v>
+      </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10</v>
       </c>
@@ -22275,8 +22579,20 @@
       <c r="AJ31" s="1">
         <v>-1.66666666667E-3</v>
       </c>
+      <c r="AO31">
+        <v>0.1</v>
+      </c>
+      <c r="AP31" s="1">
+        <v>86.902380952399994</v>
+      </c>
+      <c r="AQ31" s="1">
+        <v>86.888888888899999</v>
+      </c>
+      <c r="AR31" s="1">
+        <v>1.34920634921E-2</v>
+      </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>15</v>
       </c>
@@ -22337,8 +22653,20 @@
       <c r="AJ32" s="1">
         <v>1.66666666667E-3</v>
       </c>
+      <c r="AO32">
+        <v>0.5</v>
+      </c>
+      <c r="AP32" s="1">
+        <v>87.128571428599997</v>
+      </c>
+      <c r="AQ32" s="1">
+        <v>87.188888888899996</v>
+      </c>
+      <c r="AR32" s="1">
+        <v>-6.0317460317399998E-2</v>
+      </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20</v>
       </c>
@@ -22399,8 +22727,20 @@
       <c r="AJ33" s="1">
         <v>2.1666666666699998E-2</v>
       </c>
+      <c r="AO33">
+        <v>1</v>
+      </c>
+      <c r="AP33" s="1">
+        <v>87.138095238099993</v>
+      </c>
+      <c r="AQ33" s="1">
+        <v>87.233333333299996</v>
+      </c>
+      <c r="AR33" s="1">
+        <v>-9.5238095238100007E-2</v>
+      </c>
     </row>
-    <row r="34" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>25</v>
       </c>
@@ -22461,8 +22801,20 @@
       <c r="AJ34" s="1">
         <v>4.8333333333299998E-2</v>
       </c>
+      <c r="AO34">
+        <v>1.5</v>
+      </c>
+      <c r="AP34" s="1">
+        <v>87.161904761900004</v>
+      </c>
+      <c r="AQ34" s="1">
+        <v>87.288888888900004</v>
+      </c>
+      <c r="AR34" s="1">
+        <v>-0.126984126984</v>
+      </c>
     </row>
-    <row r="35" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>30</v>
       </c>
@@ -22523,8 +22875,20 @@
       <c r="AJ35" s="4">
         <v>-2.33333333333E-2</v>
       </c>
+      <c r="AO35">
+        <v>2</v>
+      </c>
+      <c r="AP35" s="1">
+        <v>87.1714285714</v>
+      </c>
+      <c r="AQ35" s="1">
+        <v>87.277777777799997</v>
+      </c>
+      <c r="AR35" s="1">
+        <v>-0.106349206349</v>
+      </c>
     </row>
-    <row r="36" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>40</v>
       </c>
@@ -22585,8 +22949,20 @@
       <c r="AJ36" s="1">
         <v>4.6666666666700003E-2</v>
       </c>
+      <c r="AO36">
+        <v>2.5</v>
+      </c>
+      <c r="AP36" s="1">
+        <v>87.1714285714</v>
+      </c>
+      <c r="AQ36" s="1">
+        <v>87.266666666700004</v>
+      </c>
+      <c r="AR36" s="1">
+        <v>-9.5238095238100007E-2</v>
+      </c>
     </row>
-    <row r="37" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>50</v>
       </c>
@@ -22647,8 +23023,20 @@
       <c r="AJ37" s="1">
         <v>2.1666666666699998E-2</v>
       </c>
+      <c r="AO37">
+        <v>3</v>
+      </c>
+      <c r="AP37" s="1">
+        <v>87.180952380999997</v>
+      </c>
+      <c r="AQ37" s="1">
+        <v>87.266666666700004</v>
+      </c>
+      <c r="AR37" s="1">
+        <v>-8.5714285714299995E-2</v>
+      </c>
     </row>
-    <row r="38" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>60</v>
       </c>
@@ -22709,8 +23097,20 @@
       <c r="AJ38" s="1">
         <v>5.3333333333300002E-2</v>
       </c>
+      <c r="AO38">
+        <v>3.5</v>
+      </c>
+      <c r="AP38" s="1">
+        <v>87.176190476200006</v>
+      </c>
+      <c r="AQ38" s="1">
+        <v>87.2722222222</v>
+      </c>
+      <c r="AR38" s="1">
+        <v>-9.6031746031799994E-2</v>
+      </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>70</v>
       </c>
@@ -22771,8 +23171,20 @@
       <c r="AJ39" s="1">
         <v>0.04</v>
       </c>
+      <c r="AO39">
+        <v>4</v>
+      </c>
+      <c r="AP39" s="1">
+        <v>87.183333333299998</v>
+      </c>
+      <c r="AQ39" s="1">
+        <v>87.266666666700004</v>
+      </c>
+      <c r="AR39" s="1">
+        <v>-8.3333333333299994E-2</v>
+      </c>
     </row>
-    <row r="40" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>80</v>
       </c>
@@ -22833,8 +23245,20 @@
       <c r="AJ40" s="1">
         <v>0.10833333333300001</v>
       </c>
+      <c r="AO40">
+        <v>4.5</v>
+      </c>
+      <c r="AP40" s="1">
+        <v>87.185714285700001</v>
+      </c>
+      <c r="AQ40" s="1">
+        <v>87.266666666700004</v>
+      </c>
+      <c r="AR40" s="1">
+        <v>-8.0952380952399997E-2</v>
+      </c>
     </row>
-    <row r="41" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>90</v>
       </c>
@@ -22895,8 +23319,20 @@
       <c r="AJ41" s="1">
         <v>0.05</v>
       </c>
+      <c r="AO41">
+        <v>5</v>
+      </c>
+      <c r="AP41" s="1">
+        <v>87.190476190499993</v>
+      </c>
+      <c r="AQ41" s="1">
+        <v>87.266666666700004</v>
+      </c>
+      <c r="AR41" s="1">
+        <v>-7.6190476190499998E-2</v>
+      </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>100</v>
       </c>
@@ -22957,8 +23393,20 @@
       <c r="AJ42" s="1">
         <v>-0.103333333333</v>
       </c>
+      <c r="AO42">
+        <v>6</v>
+      </c>
+      <c r="AP42" s="1">
+        <v>87.188095238100004</v>
+      </c>
+      <c r="AQ42" s="1">
+        <v>87.255555555599997</v>
+      </c>
+      <c r="AR42" s="1">
+        <v>-6.7460317460299998E-2</v>
+      </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>150</v>
       </c>
@@ -23019,8 +23467,20 @@
       <c r="AJ43" s="1">
         <v>-0.215</v>
       </c>
+      <c r="AO43">
+        <v>7</v>
+      </c>
+      <c r="AP43" s="1">
+        <v>87.188095238100004</v>
+      </c>
+      <c r="AQ43" s="1">
+        <v>87.261111111100007</v>
+      </c>
+      <c r="AR43" s="1">
+        <v>-7.3015873015899999E-2</v>
+      </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>200</v>
       </c>
@@ -23081,8 +23541,20 @@
       <c r="AJ44" s="1">
         <v>-0.178333333333</v>
       </c>
+      <c r="AO44">
+        <v>8</v>
+      </c>
+      <c r="AP44" s="1">
+        <v>87.190476190499993</v>
+      </c>
+      <c r="AQ44" s="1">
+        <v>87.261111111100007</v>
+      </c>
+      <c r="AR44" s="1">
+        <v>-7.0634920634899998E-2</v>
+      </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>250</v>
       </c>
@@ -23131,8 +23603,20 @@
       <c r="AJ45" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
+      <c r="AO45">
+        <v>9</v>
+      </c>
+      <c r="AP45" s="1">
+        <v>87.195238095199997</v>
+      </c>
+      <c r="AQ45" s="1">
+        <v>87.261111111100007</v>
+      </c>
+      <c r="AR45" s="1">
+        <v>-6.5873015872999999E-2</v>
+      </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>300</v>
       </c>
@@ -23181,8 +23665,20 @@
       <c r="AJ46" s="1">
         <v>9.6666666666699999E-2</v>
       </c>
+      <c r="AO46">
+        <v>10</v>
+      </c>
+      <c r="AP46" s="1">
+        <v>87.195238095199997</v>
+      </c>
+      <c r="AQ46" s="1">
+        <v>87.261111111100007</v>
+      </c>
+      <c r="AR46" s="1">
+        <v>-6.5873015872999999E-2</v>
+      </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>350</v>
       </c>
@@ -23231,8 +23727,20 @@
       <c r="AJ47" s="1">
         <v>-0.61666666666699999</v>
       </c>
+      <c r="AO47">
+        <v>15</v>
+      </c>
+      <c r="AP47" s="1">
+        <v>87.2</v>
+      </c>
+      <c r="AQ47" s="1">
+        <v>87.277777777799997</v>
+      </c>
+      <c r="AR47" s="1">
+        <v>-7.7777777777799997E-2</v>
+      </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>400</v>
       </c>
@@ -23290,6 +23798,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B26 B28:B51">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C26 C28:C51">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -23301,8 +23821,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C26 C28:C51">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="J2:J18 J28:J44">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -23313,7 +23833,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J18 J28:J44">
+  <conditionalFormatting sqref="K2:K18 K28:K44">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -23325,7 +23845,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K18 K28:K44">
+  <conditionalFormatting sqref="R28:R47 R2:R21">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -23337,7 +23857,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R28:R47 R2:R21">
+  <conditionalFormatting sqref="S28:S47 S2:S21">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -23349,7 +23869,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S28:S47 S2:S21">
+  <conditionalFormatting sqref="Z2:Z21 Z28:Z47">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -23361,7 +23881,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:Z21 Z28:Z47">
+  <conditionalFormatting sqref="AA28:AA47 AA2:AA21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -23373,7 +23893,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA28:AA47 AA2:AA21">
+  <conditionalFormatting sqref="AH2:AH21 AH28:AH47">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -23385,7 +23905,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH2:AH21 AH28:AH47">
+  <conditionalFormatting sqref="AI2:AI21 AI28:AI47">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -23397,7 +23917,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI2:AI21 AI28:AI47">
+  <conditionalFormatting sqref="AQ2:AQ21 AQ28:AQ47">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>